<commit_message>
modificaciones en excel a gitignore
</commit_message>
<xml_diff>
--- a/excelTaxis.xlsx
+++ b/excelTaxis.xlsx
@@ -26,13 +26,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t xml:space="preserve">1</t>
+    <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">hola</t>
+    <t xml:space="preserve">PLATE</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">dyfu</t>
   </si>
   <si>
     <t xml:space="preserve">adios</t>
@@ -369,19 +369,23 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2"/>
-      <c r="B2"/>
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>0</v>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">

</xml_diff>